<commit_message>
KP Report and KP Bill fixes
</commit_message>
<xml_diff>
--- a/docs/empty.xlsx
+++ b/docs/empty.xlsx
@@ -18,20 +18,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Here some text</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -39,8 +28,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none">
         <fgColor/>
@@ -53,8 +58,20 @@
         <bgColor/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,14 +79,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="2" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFill="true" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle builtinId="21" name="Вывод" xfId="1"/>
     <cellStyle builtinId="0" name="Обычный" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -348,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="B7:B9"/>
+  <dimension ref="A5:D5"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A7" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -360,24 +397,24 @@
     <row r="2"/>
     <row r="3"/>
     <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7" spans="2:2">
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13" spans="2:2">
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+  </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" relationships:id="rId1" orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>